<commit_message>
06.10.2024 - PART 2
</commit_message>
<xml_diff>
--- a/1__REPORT_AUTOMATION/REFERENCE_FILES/EXCL_TEST.xlsx
+++ b/1__REPORT_AUTOMATION/REFERENCE_FILES/EXCL_TEST.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westhomas/Desktop/ALFRED/1__REPORT_AUTOMATION/REFERENCE_FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9C452B-DE48-D647-BB60-6CDD194E296E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D40627B-E619-D043-9733-9E5E63919467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="880" windowWidth="34740" windowHeight="22500" activeTab="1" xr2:uid="{E496BFA4-66BC-49D0-9628-6D200FD426F9}"/>
+    <workbookView xWindow="1260" yWindow="880" windowWidth="34740" windowHeight="22500" xr2:uid="{E496BFA4-66BC-49D0-9628-6D200FD426F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="INPUT_2" sheetId="3" r:id="rId1"/>
-    <sheet name="INPUT_1" sheetId="2" r:id="rId2"/>
+    <sheet name="INPUT_1" sheetId="2" r:id="rId1"/>
+    <sheet name="INPUT_2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -432,6 +432,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931970F3-AC3E-4630-A91D-2D0AC1BCB3ED}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>IF(A2&lt;&gt;B2,VLOOKUP(A2,INPUT_2!A:B,2,0),VLOOKUP(B2,INPUT_2!A:B,2,0))</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5343B33C-F71E-462F-A6E7-59F5AD97692E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -494,45 +532,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931970F3-AC3E-4630-A91D-2D0AC1BCB3ED}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <f>IF(A2&lt;&gt;B2,VLOOKUP(A2,INPUT_2!A:B,2,0),VLOOKUP(B2,INPUT_2!A:B,2,0))</f>
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b49d9e53-0fa9-48c6-ae4e-b827f4836909" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006558401F0A96BE4BB0F9C1E3EB844901" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c79a549d573087af1da6ceb5b747f57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b49d9e53-0fa9-48c6-ae4e-b827f4836909" xmlns:ns4="da434bd8-e7d8-4f05-bd5c-7c1ec0b08732" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b00c1cc3168c7713bb0a38f65aaec641" ns3:_="" ns4:_="">
     <xsd:import namespace="b49d9e53-0fa9-48c6-ae4e-b827f4836909"/>
@@ -759,24 +776,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b49d9e53-0fa9-48c6-ae4e-b827f4836909" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CF534CB-940E-49BD-9162-3839749B4EEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="da434bd8-e7d8-4f05-bd5c-7c1ec0b08732"/>
+    <ds:schemaRef ds:uri="b49d9e53-0fa9-48c6-ae4e-b827f4836909"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F659FD-6464-4ED0-9749-22FD7F62843B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E06FC62-AAD0-4BB6-8BAB-D339E38C5417}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -793,29 +818,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04F659FD-6464-4ED0-9749-22FD7F62843B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CF534CB-940E-49BD-9162-3839749B4EEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="da434bd8-e7d8-4f05-bd5c-7c1ec0b08732"/>
-    <ds:schemaRef ds:uri="b49d9e53-0fa9-48c6-ae4e-b827f4836909"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>